<commit_message>
Updated Excel with resources thumbs
</commit_message>
<xml_diff>
--- a/resources/excel/resources.xlsx
+++ b/resources/excel/resources.xlsx
@@ -2433,8 +2433,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF987"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B21" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+    <sheetView tabSelected="1" topLeftCell="B21" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>

</xml_diff>